<commit_message>
updated website and created .py files
</commit_message>
<xml_diff>
--- a/data/albumdata.xlsx
+++ b/data/albumdata.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sammo\OneDrive\Desktop\digit494\bobdylan494\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{026891FF-0A42-45A5-B91A-827C7312818F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25884243-20E9-47C1-B7A2-72AE3FF440F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{FEEBB7A0-F159-473C-BB2C-0727624CED14}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{FEEBB7A0-F159-473C-BB2C-0727624CED14}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="live-comp albums" sheetId="3" r:id="rId3"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId2"/>
+    <externalReference r:id="rId4"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="87">
   <si>
     <t>AlbumName</t>
   </si>
@@ -279,6 +281,27 @@
   </si>
   <si>
     <t>TrackCount</t>
+  </si>
+  <si>
+    <t>Late Dylan</t>
+  </si>
+  <si>
+    <t>Early Dylan</t>
+  </si>
+  <si>
+    <t>Period</t>
+  </si>
+  <si>
+    <t>Release Year</t>
+  </si>
+  <si>
+    <t>Total #of Albums</t>
+  </si>
+  <si>
+    <t>AlbumType</t>
+  </si>
+  <si>
+    <t>Live</t>
   </si>
 </sst>
 </file>
@@ -333,6 +356,866 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'live-comp albums'!$J$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total #of Albums</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'live-comp albums'!$I$5:$I$6</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Early Dylan</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Late Dylan</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'live-comp albums'!$J$5:$J$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>34</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-343A-4199-8100-1BF19B12A264}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="182"/>
+        <c:axId val="1231727471"/>
+        <c:axId val="1231723151"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1231727471"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1231723151"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1231723151"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1231727471"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>68580</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>156210</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>373380</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>156210</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0009ADDB-A884-BE70-DD3F-E442E0D2CCF1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1505,10 +2388,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76129176-828D-47B7-819F-0A41AB8CCC8C}">
-  <dimension ref="A1:E76"/>
+  <dimension ref="A1:F76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="H69" sqref="H69"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1519,7 +2402,7 @@
     <col min="5" max="5" width="11.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1535,8 +2418,11 @@
       <c r="E1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1554,8 +2440,12 @@
       <c r="E2">
         <v>2023</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F2" t="str">
+        <f>IF(E2&lt;1980,"Early Dylan","Late Dylan")</f>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1573,8 +2463,12 @@
       <c r="E3">
         <v>2023</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F3" t="str">
+        <f t="shared" ref="F3:F66" si="0">IF(E3&lt;1980,"Early Dylan","Late Dylan")</f>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1592,8 +2486,12 @@
       <c r="E4">
         <v>2021</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F4" t="str">
+        <f t="shared" si="0"/>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1611,8 +2509,12 @@
       <c r="E5">
         <v>2021</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F5" t="str">
+        <f t="shared" si="0"/>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -1630,8 +2532,12 @@
       <c r="E6">
         <v>2021</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F6" t="str">
+        <f t="shared" si="0"/>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -1649,8 +2555,12 @@
       <c r="E7">
         <v>2020</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F7" t="str">
+        <f t="shared" si="0"/>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -1668,8 +2578,12 @@
       <c r="E8">
         <v>2020</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F8" t="str">
+        <f t="shared" si="0"/>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -1687,8 +2601,12 @@
       <c r="E9">
         <v>2019</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F9" t="str">
+        <f t="shared" si="0"/>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -1706,8 +2624,12 @@
       <c r="E10">
         <v>2019</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F10" t="str">
+        <f t="shared" si="0"/>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -1725,8 +2647,12 @@
       <c r="E11">
         <v>2018</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F11" t="str">
+        <f t="shared" si="0"/>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -1744,8 +2670,12 @@
       <c r="E12">
         <v>2017</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F12" t="str">
+        <f t="shared" si="0"/>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -1763,8 +2693,12 @@
       <c r="E13">
         <v>2017</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F13" t="str">
+        <f t="shared" si="0"/>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -1782,8 +2716,12 @@
       <c r="E14">
         <v>2016</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F14" t="str">
+        <f t="shared" si="0"/>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -1801,8 +2739,12 @@
       <c r="E15">
         <v>2015</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F15" t="str">
+        <f t="shared" si="0"/>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -1820,8 +2762,12 @@
       <c r="E16">
         <v>2015</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F16" t="str">
+        <f t="shared" si="0"/>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -1839,8 +2785,12 @@
       <c r="E17">
         <v>2013</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F17" t="str">
+        <f t="shared" si="0"/>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -1858,8 +2808,12 @@
       <c r="E18">
         <v>2012</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F18" t="str">
+        <f t="shared" si="0"/>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -1877,8 +2831,12 @@
       <c r="E19">
         <v>2011</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F19" t="str">
+        <f t="shared" si="0"/>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -1896,8 +2854,12 @@
       <c r="E20">
         <v>2010</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F20" t="str">
+        <f t="shared" si="0"/>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -1915,8 +2877,12 @@
       <c r="E21">
         <v>2009</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F21" t="str">
+        <f t="shared" si="0"/>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -1934,8 +2900,12 @@
       <c r="E22">
         <v>2009</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F22" t="str">
+        <f t="shared" si="0"/>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -1953,8 +2923,12 @@
       <c r="E23">
         <v>2008</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F23" t="str">
+        <f t="shared" si="0"/>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>25</v>
       </c>
@@ -1972,8 +2946,12 @@
       <c r="E24">
         <v>2006</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F24" t="str">
+        <f t="shared" si="0"/>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -1991,8 +2969,12 @@
       <c r="E25">
         <v>2005</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F25" t="str">
+        <f t="shared" si="0"/>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>27</v>
       </c>
@@ -2010,8 +2992,12 @@
       <c r="E26">
         <v>2005</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F26" t="str">
+        <f t="shared" si="0"/>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>28</v>
       </c>
@@ -2029,8 +3015,12 @@
       <c r="E27">
         <v>2005</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F27" t="str">
+        <f t="shared" si="0"/>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>29</v>
       </c>
@@ -2048,8 +3038,12 @@
       <c r="E28">
         <v>2004</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F28" t="str">
+        <f t="shared" si="0"/>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>30</v>
       </c>
@@ -2067,8 +3061,12 @@
       <c r="E29">
         <v>2002</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F29" t="str">
+        <f t="shared" si="0"/>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>31</v>
       </c>
@@ -2086,8 +3084,12 @@
       <c r="E30">
         <v>2002</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F30" t="str">
+        <f t="shared" si="0"/>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>32</v>
       </c>
@@ -2105,8 +3107,12 @@
       <c r="E31">
         <v>2001</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F31" t="str">
+        <f t="shared" si="0"/>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>33</v>
       </c>
@@ -2124,8 +3130,12 @@
       <c r="E32">
         <v>1998</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F32" t="str">
+        <f t="shared" si="0"/>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>34</v>
       </c>
@@ -2143,8 +3153,12 @@
       <c r="E33">
         <v>1997</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F33" t="str">
+        <f t="shared" si="0"/>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>35</v>
       </c>
@@ -2162,8 +3176,12 @@
       <c r="E34">
         <v>1995</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F34" t="str">
+        <f t="shared" si="0"/>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>36</v>
       </c>
@@ -2181,8 +3199,12 @@
       <c r="E35">
         <v>1994</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F35" t="str">
+        <f t="shared" si="0"/>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>37</v>
       </c>
@@ -2200,8 +3222,12 @@
       <c r="E36">
         <v>1994</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F36" t="str">
+        <f t="shared" si="0"/>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>38</v>
       </c>
@@ -2219,8 +3245,12 @@
       <c r="E37">
         <v>1993</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F37" t="str">
+        <f t="shared" si="0"/>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>39</v>
       </c>
@@ -2238,8 +3268,12 @@
       <c r="E38">
         <v>1992</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F38" t="str">
+        <f t="shared" si="0"/>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>40</v>
       </c>
@@ -2257,8 +3291,12 @@
       <c r="E39">
         <v>1991</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F39" t="str">
+        <f t="shared" si="0"/>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>41</v>
       </c>
@@ -2276,8 +3314,12 @@
       <c r="E40">
         <v>1990</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F40" t="str">
+        <f t="shared" si="0"/>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>42</v>
       </c>
@@ -2295,8 +3337,12 @@
       <c r="E41">
         <v>1989</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F41" t="str">
+        <f t="shared" si="0"/>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>43</v>
       </c>
@@ -2314,8 +3360,12 @@
       <c r="E42">
         <v>1988</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F42" t="str">
+        <f t="shared" si="0"/>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>44</v>
       </c>
@@ -2333,8 +3383,12 @@
       <c r="E43">
         <v>1986</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F43" t="str">
+        <f t="shared" si="0"/>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>45</v>
       </c>
@@ -2352,8 +3406,12 @@
       <c r="E44">
         <v>1985</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F44" t="str">
+        <f t="shared" si="0"/>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>46</v>
       </c>
@@ -2371,8 +3429,12 @@
       <c r="E45">
         <v>1985</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F45" t="str">
+        <f t="shared" si="0"/>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>47</v>
       </c>
@@ -2390,8 +3452,12 @@
       <c r="E46">
         <v>1984</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F46" t="str">
+        <f t="shared" si="0"/>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>48</v>
       </c>
@@ -2409,8 +3475,12 @@
       <c r="E47">
         <v>1983</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F47" t="str">
+        <f t="shared" si="0"/>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>49</v>
       </c>
@@ -2428,8 +3498,12 @@
       <c r="E48">
         <v>1981</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F48" t="str">
+        <f t="shared" si="0"/>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>50</v>
       </c>
@@ -2447,8 +3521,12 @@
       <c r="E49">
         <v>1980</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F49" t="str">
+        <f t="shared" si="0"/>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>51</v>
       </c>
@@ -2466,8 +3544,12 @@
       <c r="E50">
         <v>1979</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F50" t="str">
+        <f t="shared" si="0"/>
+        <v>Early Dylan</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>52</v>
       </c>
@@ -2485,8 +3567,12 @@
       <c r="E51">
         <v>1979</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F51" t="str">
+        <f t="shared" si="0"/>
+        <v>Early Dylan</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>53</v>
       </c>
@@ -2504,8 +3590,12 @@
       <c r="E52">
         <v>1978</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F52" t="str">
+        <f t="shared" si="0"/>
+        <v>Early Dylan</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>54</v>
       </c>
@@ -2523,8 +3613,12 @@
       <c r="E53">
         <v>1978</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F53" t="str">
+        <f t="shared" si="0"/>
+        <v>Early Dylan</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>55</v>
       </c>
@@ -2542,8 +3636,12 @@
       <c r="E54">
         <v>1976</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F54" t="str">
+        <f t="shared" si="0"/>
+        <v>Early Dylan</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>56</v>
       </c>
@@ -2561,8 +3659,12 @@
       <c r="E55">
         <v>1976</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F55" t="str">
+        <f t="shared" si="0"/>
+        <v>Early Dylan</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>57</v>
       </c>
@@ -2580,8 +3682,12 @@
       <c r="E56">
         <v>1975</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F56" t="str">
+        <f t="shared" si="0"/>
+        <v>Early Dylan</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>58</v>
       </c>
@@ -2599,8 +3705,12 @@
       <c r="E57">
         <v>1974</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F57" t="str">
+        <f t="shared" si="0"/>
+        <v>Early Dylan</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>59</v>
       </c>
@@ -2618,8 +3728,12 @@
       <c r="E58">
         <v>1973</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F58" t="str">
+        <f t="shared" si="0"/>
+        <v>Early Dylan</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>60</v>
       </c>
@@ -2637,8 +3751,12 @@
       <c r="E59">
         <v>1973</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F59" t="str">
+        <f t="shared" si="0"/>
+        <v>Early Dylan</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>61</v>
       </c>
@@ -2656,8 +3774,12 @@
       <c r="E60">
         <v>1971</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F60" t="str">
+        <f t="shared" si="0"/>
+        <v>Early Dylan</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>62</v>
       </c>
@@ -2675,8 +3797,12 @@
       <c r="E61">
         <v>1970</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F61" t="str">
+        <f t="shared" si="0"/>
+        <v>Early Dylan</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>63</v>
       </c>
@@ -2694,8 +3820,12 @@
       <c r="E62">
         <v>1970</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F62" t="str">
+        <f t="shared" si="0"/>
+        <v>Early Dylan</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>64</v>
       </c>
@@ -2713,8 +3843,12 @@
       <c r="E63">
         <v>1969</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F63" t="str">
+        <f t="shared" si="0"/>
+        <v>Early Dylan</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>65</v>
       </c>
@@ -2732,8 +3866,12 @@
       <c r="E64">
         <v>1967</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F64" t="str">
+        <f t="shared" si="0"/>
+        <v>Early Dylan</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>66</v>
       </c>
@@ -2751,8 +3889,12 @@
       <c r="E65">
         <v>1967</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F65" t="str">
+        <f t="shared" si="0"/>
+        <v>Early Dylan</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>67</v>
       </c>
@@ -2770,8 +3912,12 @@
       <c r="E66">
         <v>1966</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F66" t="str">
+        <f t="shared" si="0"/>
+        <v>Early Dylan</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>68</v>
       </c>
@@ -2789,8 +3935,12 @@
       <c r="E67">
         <v>1965</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F67" t="str">
+        <f t="shared" ref="F67:F72" si="1">IF(E67&lt;1980,"Early Dylan","Late Dylan")</f>
+        <v>Early Dylan</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>69</v>
       </c>
@@ -2808,8 +3958,12 @@
       <c r="E68">
         <v>1965</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F68" t="str">
+        <f t="shared" si="1"/>
+        <v>Early Dylan</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>70</v>
       </c>
@@ -2827,8 +3981,12 @@
       <c r="E69">
         <v>1964</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F69" t="str">
+        <f t="shared" si="1"/>
+        <v>Early Dylan</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>71</v>
       </c>
@@ -2846,8 +4004,12 @@
       <c r="E70">
         <v>1964</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F70" t="str">
+        <f t="shared" si="1"/>
+        <v>Early Dylan</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>72</v>
       </c>
@@ -2865,8 +4027,12 @@
       <c r="E71">
         <v>1963</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F71" t="str">
+        <f t="shared" si="1"/>
+        <v>Early Dylan</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>73</v>
       </c>
@@ -2884,8 +4050,12 @@
       <c r="E72">
         <v>1962</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F72" t="str">
+        <f t="shared" si="1"/>
+        <v>Early Dylan</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>74</v>
       </c>
@@ -2898,7 +4068,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>75</v>
       </c>
@@ -2911,7 +4081,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>76</v>
       </c>
@@ -2924,7 +4094,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>77</v>
       </c>
@@ -2940,4 +4110,1294 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D4560C7-A3C3-4630-84F1-BFF97B1BE306}">
+  <dimension ref="C1:Q72"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P1" sqref="P1:Q1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="16" max="16" width="11.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="P1" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="P2">
+        <v>2023</v>
+      </c>
+      <c r="Q2" t="str">
+        <f>IF(P2&lt;1980,"Early Dylan","Late Dylan")</f>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="3" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D3">
+        <v>48</v>
+      </c>
+      <c r="P3">
+        <v>2023</v>
+      </c>
+      <c r="Q3" t="str">
+        <f t="shared" ref="Q3:Q66" si="0">IF(P3&lt;1980,"Early Dylan","Late Dylan")</f>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="4" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D4">
+        <v>23</v>
+      </c>
+      <c r="P4">
+        <v>2021</v>
+      </c>
+      <c r="Q4" t="str">
+        <f t="shared" si="0"/>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="5" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="D5">
+        <f>SUM(D3:D4)</f>
+        <v>71</v>
+      </c>
+      <c r="P5">
+        <v>2021</v>
+      </c>
+      <c r="Q5" t="str">
+        <f t="shared" si="0"/>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="6" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="P6">
+        <v>2021</v>
+      </c>
+      <c r="Q6" t="str">
+        <f t="shared" si="0"/>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="7" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="P7">
+        <v>2020</v>
+      </c>
+      <c r="Q7" t="str">
+        <f t="shared" si="0"/>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="8" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="P8">
+        <v>2020</v>
+      </c>
+      <c r="Q8" t="str">
+        <f t="shared" si="0"/>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="9" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="P9">
+        <v>2019</v>
+      </c>
+      <c r="Q9" t="str">
+        <f t="shared" si="0"/>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="10" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="P10">
+        <v>2019</v>
+      </c>
+      <c r="Q10" t="str">
+        <f t="shared" si="0"/>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="11" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="P11">
+        <v>2018</v>
+      </c>
+      <c r="Q11" t="str">
+        <f t="shared" si="0"/>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="12" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="P12">
+        <v>2017</v>
+      </c>
+      <c r="Q12" t="str">
+        <f t="shared" si="0"/>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="13" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="P13">
+        <v>2017</v>
+      </c>
+      <c r="Q13" t="str">
+        <f t="shared" si="0"/>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="14" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="P14">
+        <v>2016</v>
+      </c>
+      <c r="Q14" t="str">
+        <f t="shared" si="0"/>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="15" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="P15">
+        <v>2015</v>
+      </c>
+      <c r="Q15" t="str">
+        <f t="shared" si="0"/>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="16" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="P16">
+        <v>2015</v>
+      </c>
+      <c r="Q16" t="str">
+        <f t="shared" si="0"/>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="17" spans="16:17" x14ac:dyDescent="0.3">
+      <c r="P17">
+        <v>2013</v>
+      </c>
+      <c r="Q17" t="str">
+        <f t="shared" si="0"/>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="18" spans="16:17" x14ac:dyDescent="0.3">
+      <c r="P18">
+        <v>2012</v>
+      </c>
+      <c r="Q18" t="str">
+        <f t="shared" si="0"/>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="19" spans="16:17" x14ac:dyDescent="0.3">
+      <c r="P19">
+        <v>2011</v>
+      </c>
+      <c r="Q19" t="str">
+        <f t="shared" si="0"/>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="20" spans="16:17" x14ac:dyDescent="0.3">
+      <c r="P20">
+        <v>2010</v>
+      </c>
+      <c r="Q20" t="str">
+        <f t="shared" si="0"/>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="21" spans="16:17" x14ac:dyDescent="0.3">
+      <c r="P21">
+        <v>2009</v>
+      </c>
+      <c r="Q21" t="str">
+        <f t="shared" si="0"/>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="22" spans="16:17" x14ac:dyDescent="0.3">
+      <c r="P22">
+        <v>2009</v>
+      </c>
+      <c r="Q22" t="str">
+        <f t="shared" si="0"/>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="23" spans="16:17" x14ac:dyDescent="0.3">
+      <c r="P23">
+        <v>2008</v>
+      </c>
+      <c r="Q23" t="str">
+        <f t="shared" si="0"/>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="24" spans="16:17" x14ac:dyDescent="0.3">
+      <c r="P24">
+        <v>2006</v>
+      </c>
+      <c r="Q24" t="str">
+        <f t="shared" si="0"/>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="25" spans="16:17" x14ac:dyDescent="0.3">
+      <c r="P25">
+        <v>2005</v>
+      </c>
+      <c r="Q25" t="str">
+        <f t="shared" si="0"/>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="26" spans="16:17" x14ac:dyDescent="0.3">
+      <c r="P26">
+        <v>2005</v>
+      </c>
+      <c r="Q26" t="str">
+        <f t="shared" si="0"/>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="27" spans="16:17" x14ac:dyDescent="0.3">
+      <c r="P27">
+        <v>2005</v>
+      </c>
+      <c r="Q27" t="str">
+        <f t="shared" si="0"/>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="28" spans="16:17" x14ac:dyDescent="0.3">
+      <c r="P28">
+        <v>2004</v>
+      </c>
+      <c r="Q28" t="str">
+        <f t="shared" si="0"/>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="29" spans="16:17" x14ac:dyDescent="0.3">
+      <c r="P29">
+        <v>2002</v>
+      </c>
+      <c r="Q29" t="str">
+        <f t="shared" si="0"/>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="30" spans="16:17" x14ac:dyDescent="0.3">
+      <c r="P30">
+        <v>2002</v>
+      </c>
+      <c r="Q30" t="str">
+        <f t="shared" si="0"/>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="31" spans="16:17" x14ac:dyDescent="0.3">
+      <c r="P31">
+        <v>2001</v>
+      </c>
+      <c r="Q31" t="str">
+        <f t="shared" si="0"/>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="32" spans="16:17" x14ac:dyDescent="0.3">
+      <c r="P32">
+        <v>1998</v>
+      </c>
+      <c r="Q32" t="str">
+        <f t="shared" si="0"/>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="33" spans="16:17" x14ac:dyDescent="0.3">
+      <c r="P33">
+        <v>1997</v>
+      </c>
+      <c r="Q33" t="str">
+        <f t="shared" si="0"/>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="34" spans="16:17" x14ac:dyDescent="0.3">
+      <c r="P34">
+        <v>1995</v>
+      </c>
+      <c r="Q34" t="str">
+        <f t="shared" si="0"/>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="35" spans="16:17" x14ac:dyDescent="0.3">
+      <c r="P35">
+        <v>1994</v>
+      </c>
+      <c r="Q35" t="str">
+        <f t="shared" si="0"/>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="36" spans="16:17" x14ac:dyDescent="0.3">
+      <c r="P36">
+        <v>1994</v>
+      </c>
+      <c r="Q36" t="str">
+        <f t="shared" si="0"/>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="37" spans="16:17" x14ac:dyDescent="0.3">
+      <c r="P37">
+        <v>1993</v>
+      </c>
+      <c r="Q37" t="str">
+        <f t="shared" si="0"/>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="38" spans="16:17" x14ac:dyDescent="0.3">
+      <c r="P38">
+        <v>1992</v>
+      </c>
+      <c r="Q38" t="str">
+        <f t="shared" si="0"/>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="39" spans="16:17" x14ac:dyDescent="0.3">
+      <c r="P39">
+        <v>1991</v>
+      </c>
+      <c r="Q39" t="str">
+        <f t="shared" si="0"/>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="40" spans="16:17" x14ac:dyDescent="0.3">
+      <c r="P40">
+        <v>1990</v>
+      </c>
+      <c r="Q40" t="str">
+        <f t="shared" si="0"/>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="41" spans="16:17" x14ac:dyDescent="0.3">
+      <c r="P41">
+        <v>1989</v>
+      </c>
+      <c r="Q41" t="str">
+        <f t="shared" si="0"/>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="42" spans="16:17" x14ac:dyDescent="0.3">
+      <c r="P42">
+        <v>1988</v>
+      </c>
+      <c r="Q42" t="str">
+        <f t="shared" si="0"/>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="43" spans="16:17" x14ac:dyDescent="0.3">
+      <c r="P43">
+        <v>1986</v>
+      </c>
+      <c r="Q43" t="str">
+        <f t="shared" si="0"/>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="44" spans="16:17" x14ac:dyDescent="0.3">
+      <c r="P44">
+        <v>1985</v>
+      </c>
+      <c r="Q44" t="str">
+        <f t="shared" si="0"/>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="45" spans="16:17" x14ac:dyDescent="0.3">
+      <c r="P45">
+        <v>1985</v>
+      </c>
+      <c r="Q45" t="str">
+        <f t="shared" si="0"/>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="46" spans="16:17" x14ac:dyDescent="0.3">
+      <c r="P46">
+        <v>1984</v>
+      </c>
+      <c r="Q46" t="str">
+        <f t="shared" si="0"/>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="47" spans="16:17" x14ac:dyDescent="0.3">
+      <c r="P47">
+        <v>1983</v>
+      </c>
+      <c r="Q47" t="str">
+        <f t="shared" si="0"/>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="48" spans="16:17" x14ac:dyDescent="0.3">
+      <c r="P48">
+        <v>1981</v>
+      </c>
+      <c r="Q48" t="str">
+        <f t="shared" si="0"/>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="49" spans="16:17" x14ac:dyDescent="0.3">
+      <c r="P49">
+        <v>1980</v>
+      </c>
+      <c r="Q49" t="str">
+        <f t="shared" si="0"/>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="50" spans="16:17" x14ac:dyDescent="0.3">
+      <c r="P50">
+        <v>1979</v>
+      </c>
+      <c r="Q50" t="str">
+        <f t="shared" si="0"/>
+        <v>Early Dylan</v>
+      </c>
+    </row>
+    <row r="51" spans="16:17" x14ac:dyDescent="0.3">
+      <c r="P51">
+        <v>1979</v>
+      </c>
+      <c r="Q51" t="str">
+        <f t="shared" si="0"/>
+        <v>Early Dylan</v>
+      </c>
+    </row>
+    <row r="52" spans="16:17" x14ac:dyDescent="0.3">
+      <c r="P52">
+        <v>1978</v>
+      </c>
+      <c r="Q52" t="str">
+        <f t="shared" si="0"/>
+        <v>Early Dylan</v>
+      </c>
+    </row>
+    <row r="53" spans="16:17" x14ac:dyDescent="0.3">
+      <c r="P53">
+        <v>1978</v>
+      </c>
+      <c r="Q53" t="str">
+        <f t="shared" si="0"/>
+        <v>Early Dylan</v>
+      </c>
+    </row>
+    <row r="54" spans="16:17" x14ac:dyDescent="0.3">
+      <c r="P54">
+        <v>1976</v>
+      </c>
+      <c r="Q54" t="str">
+        <f t="shared" si="0"/>
+        <v>Early Dylan</v>
+      </c>
+    </row>
+    <row r="55" spans="16:17" x14ac:dyDescent="0.3">
+      <c r="P55">
+        <v>1976</v>
+      </c>
+      <c r="Q55" t="str">
+        <f t="shared" si="0"/>
+        <v>Early Dylan</v>
+      </c>
+    </row>
+    <row r="56" spans="16:17" x14ac:dyDescent="0.3">
+      <c r="P56">
+        <v>1975</v>
+      </c>
+      <c r="Q56" t="str">
+        <f t="shared" si="0"/>
+        <v>Early Dylan</v>
+      </c>
+    </row>
+    <row r="57" spans="16:17" x14ac:dyDescent="0.3">
+      <c r="P57">
+        <v>1974</v>
+      </c>
+      <c r="Q57" t="str">
+        <f t="shared" si="0"/>
+        <v>Early Dylan</v>
+      </c>
+    </row>
+    <row r="58" spans="16:17" x14ac:dyDescent="0.3">
+      <c r="P58">
+        <v>1973</v>
+      </c>
+      <c r="Q58" t="str">
+        <f t="shared" si="0"/>
+        <v>Early Dylan</v>
+      </c>
+    </row>
+    <row r="59" spans="16:17" x14ac:dyDescent="0.3">
+      <c r="P59">
+        <v>1973</v>
+      </c>
+      <c r="Q59" t="str">
+        <f t="shared" si="0"/>
+        <v>Early Dylan</v>
+      </c>
+    </row>
+    <row r="60" spans="16:17" x14ac:dyDescent="0.3">
+      <c r="P60">
+        <v>1971</v>
+      </c>
+      <c r="Q60" t="str">
+        <f t="shared" si="0"/>
+        <v>Early Dylan</v>
+      </c>
+    </row>
+    <row r="61" spans="16:17" x14ac:dyDescent="0.3">
+      <c r="P61">
+        <v>1970</v>
+      </c>
+      <c r="Q61" t="str">
+        <f t="shared" si="0"/>
+        <v>Early Dylan</v>
+      </c>
+    </row>
+    <row r="62" spans="16:17" x14ac:dyDescent="0.3">
+      <c r="P62">
+        <v>1970</v>
+      </c>
+      <c r="Q62" t="str">
+        <f t="shared" si="0"/>
+        <v>Early Dylan</v>
+      </c>
+    </row>
+    <row r="63" spans="16:17" x14ac:dyDescent="0.3">
+      <c r="P63">
+        <v>1969</v>
+      </c>
+      <c r="Q63" t="str">
+        <f t="shared" si="0"/>
+        <v>Early Dylan</v>
+      </c>
+    </row>
+    <row r="64" spans="16:17" x14ac:dyDescent="0.3">
+      <c r="P64">
+        <v>1967</v>
+      </c>
+      <c r="Q64" t="str">
+        <f t="shared" si="0"/>
+        <v>Early Dylan</v>
+      </c>
+    </row>
+    <row r="65" spans="16:17" x14ac:dyDescent="0.3">
+      <c r="P65">
+        <v>1967</v>
+      </c>
+      <c r="Q65" t="str">
+        <f t="shared" si="0"/>
+        <v>Early Dylan</v>
+      </c>
+    </row>
+    <row r="66" spans="16:17" x14ac:dyDescent="0.3">
+      <c r="P66">
+        <v>1966</v>
+      </c>
+      <c r="Q66" t="str">
+        <f t="shared" si="0"/>
+        <v>Early Dylan</v>
+      </c>
+    </row>
+    <row r="67" spans="16:17" x14ac:dyDescent="0.3">
+      <c r="P67">
+        <v>1965</v>
+      </c>
+      <c r="Q67" t="str">
+        <f t="shared" ref="Q67:Q72" si="1">IF(P67&lt;1980,"Early Dylan","Late Dylan")</f>
+        <v>Early Dylan</v>
+      </c>
+    </row>
+    <row r="68" spans="16:17" x14ac:dyDescent="0.3">
+      <c r="P68">
+        <v>1965</v>
+      </c>
+      <c r="Q68" t="str">
+        <f t="shared" si="1"/>
+        <v>Early Dylan</v>
+      </c>
+    </row>
+    <row r="69" spans="16:17" x14ac:dyDescent="0.3">
+      <c r="P69">
+        <v>1964</v>
+      </c>
+      <c r="Q69" t="str">
+        <f t="shared" si="1"/>
+        <v>Early Dylan</v>
+      </c>
+    </row>
+    <row r="70" spans="16:17" x14ac:dyDescent="0.3">
+      <c r="P70">
+        <v>1964</v>
+      </c>
+      <c r="Q70" t="str">
+        <f t="shared" si="1"/>
+        <v>Early Dylan</v>
+      </c>
+    </row>
+    <row r="71" spans="16:17" x14ac:dyDescent="0.3">
+      <c r="P71">
+        <v>1963</v>
+      </c>
+      <c r="Q71" t="str">
+        <f t="shared" si="1"/>
+        <v>Early Dylan</v>
+      </c>
+    </row>
+    <row r="72" spans="16:17" x14ac:dyDescent="0.3">
+      <c r="P72">
+        <v>1962</v>
+      </c>
+      <c r="Q72" t="str">
+        <f t="shared" si="1"/>
+        <v>Early Dylan</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C5F1180-7C84-4933-920D-C045A2DDB9BC}">
+  <dimension ref="A1:J44"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="73" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <f>VLOOKUP(A:A,Sheet1!A:F,5,FALSE)</f>
+        <v>2023</v>
+      </c>
+      <c r="C2" t="str">
+        <f>VLOOKUP(A:A,Sheet1!A:F,6,FALSE)</f>
+        <v>Late Dylan</v>
+      </c>
+      <c r="D2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <f>VLOOKUP(A:A,Sheet1!A:F,5,FALSE)</f>
+        <v>2023</v>
+      </c>
+      <c r="C3" t="str">
+        <f>VLOOKUP(A:A,Sheet1!A:F,6,FALSE)</f>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <f>VLOOKUP(A:A,Sheet1!A:F,5,FALSE)</f>
+        <v>2021</v>
+      </c>
+      <c r="C4" t="str">
+        <f>VLOOKUP(A:A,Sheet1!A:F,6,FALSE)</f>
+        <v>Late Dylan</v>
+      </c>
+      <c r="J4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <f>VLOOKUP(A:A,Sheet1!A:F,5,FALSE)</f>
+        <v>2021</v>
+      </c>
+      <c r="C5" t="str">
+        <f>VLOOKUP(A:A,Sheet1!A:F,6,FALSE)</f>
+        <v>Late Dylan</v>
+      </c>
+      <c r="I5" t="s">
+        <v>81</v>
+      </c>
+      <c r="J5">
+        <f>COUNTIF(C2:C44,"Early Dylan")</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <f>VLOOKUP(A:A,Sheet1!A:F,5,FALSE)</f>
+        <v>2021</v>
+      </c>
+      <c r="C6" t="str">
+        <f>VLOOKUP(A:A,Sheet1!A:F,6,FALSE)</f>
+        <v>Late Dylan</v>
+      </c>
+      <c r="I6" t="s">
+        <v>80</v>
+      </c>
+      <c r="J6">
+        <f>COUNTIF(C2:C45,"Late Dylan")</f>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7">
+        <f>VLOOKUP(A:A,Sheet1!A:F,5,FALSE)</f>
+        <v>2020</v>
+      </c>
+      <c r="C7" t="str">
+        <f>VLOOKUP(A:A,Sheet1!A:F,6,FALSE)</f>
+        <v>Late Dylan</v>
+      </c>
+      <c r="J7">
+        <f>SUM(J5:J6)</f>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8">
+        <f>VLOOKUP(A:A,Sheet1!A:F,5,FALSE)</f>
+        <v>2019</v>
+      </c>
+      <c r="C8" t="str">
+        <f>VLOOKUP(A:A,Sheet1!A:F,6,FALSE)</f>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9">
+        <f>VLOOKUP(A:A,Sheet1!A:F,5,FALSE)</f>
+        <v>2019</v>
+      </c>
+      <c r="C9" t="str">
+        <f>VLOOKUP(A:A,Sheet1!A:F,6,FALSE)</f>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10">
+        <f>VLOOKUP(A:A,Sheet1!A:F,5,FALSE)</f>
+        <v>2018</v>
+      </c>
+      <c r="C10" t="str">
+        <f>VLOOKUP(A:A,Sheet1!A:F,6,FALSE)</f>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11">
+        <f>VLOOKUP(A:A,Sheet1!A:F,5,FALSE)</f>
+        <v>2017</v>
+      </c>
+      <c r="C11" t="str">
+        <f>VLOOKUP(A:A,Sheet1!A:F,6,FALSE)</f>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12">
+        <f>VLOOKUP(A:A,Sheet1!A:F,5,FALSE)</f>
+        <v>2017</v>
+      </c>
+      <c r="C12" t="str">
+        <f>VLOOKUP(A:A,Sheet1!A:F,6,FALSE)</f>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13">
+        <f>VLOOKUP(A:A,Sheet1!A:F,5,FALSE)</f>
+        <v>2016</v>
+      </c>
+      <c r="C13" t="str">
+        <f>VLOOKUP(A:A,Sheet1!A:F,6,FALSE)</f>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14">
+        <f>VLOOKUP(A:A,Sheet1!A:F,5,FALSE)</f>
+        <v>2015</v>
+      </c>
+      <c r="C14" t="str">
+        <f>VLOOKUP(A:A,Sheet1!A:F,6,FALSE)</f>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15">
+        <f>VLOOKUP(A:A,Sheet1!A:F,5,FALSE)</f>
+        <v>2015</v>
+      </c>
+      <c r="C15" t="str">
+        <f>VLOOKUP(A:A,Sheet1!A:F,6,FALSE)</f>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16">
+        <f>VLOOKUP(A:A,Sheet1!A:F,5,FALSE)</f>
+        <v>2013</v>
+      </c>
+      <c r="C16" t="str">
+        <f>VLOOKUP(A:A,Sheet1!A:F,6,FALSE)</f>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17">
+        <f>VLOOKUP(A:A,Sheet1!A:F,5,FALSE)</f>
+        <v>2011</v>
+      </c>
+      <c r="C17" t="str">
+        <f>VLOOKUP(A:A,Sheet1!A:F,6,FALSE)</f>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18">
+        <f>VLOOKUP(A:A,Sheet1!A:F,5,FALSE)</f>
+        <v>2010</v>
+      </c>
+      <c r="C18" t="str">
+        <f>VLOOKUP(A:A,Sheet1!A:F,6,FALSE)</f>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19">
+        <f>VLOOKUP(A:A,Sheet1!A:F,5,FALSE)</f>
+        <v>2009</v>
+      </c>
+      <c r="C19" t="str">
+        <f>VLOOKUP(A:A,Sheet1!A:F,6,FALSE)</f>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20">
+        <f>VLOOKUP(A:A,Sheet1!A:F,5,FALSE)</f>
+        <v>2008</v>
+      </c>
+      <c r="C20" t="str">
+        <f>VLOOKUP(A:A,Sheet1!A:F,6,FALSE)</f>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21">
+        <f>VLOOKUP(A:A,Sheet1!A:F,5,FALSE)</f>
+        <v>2005</v>
+      </c>
+      <c r="C21" t="str">
+        <f>VLOOKUP(A:A,Sheet1!A:F,6,FALSE)</f>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22">
+        <f>VLOOKUP(A:A,Sheet1!A:F,5,FALSE)</f>
+        <v>2005</v>
+      </c>
+      <c r="C22" t="str">
+        <f>VLOOKUP(A:A,Sheet1!A:F,6,FALSE)</f>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23">
+        <f>VLOOKUP(A:A,Sheet1!A:F,5,FALSE)</f>
+        <v>2005</v>
+      </c>
+      <c r="C23" t="str">
+        <f>VLOOKUP(A:A,Sheet1!A:F,6,FALSE)</f>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24">
+        <f>VLOOKUP(A:A,Sheet1!A:F,5,FALSE)</f>
+        <v>2004</v>
+      </c>
+      <c r="C24" t="str">
+        <f>VLOOKUP(A:A,Sheet1!A:F,6,FALSE)</f>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>30</v>
+      </c>
+      <c r="B25">
+        <f>VLOOKUP(A:A,Sheet1!A:F,5,FALSE)</f>
+        <v>2002</v>
+      </c>
+      <c r="C25" t="str">
+        <f>VLOOKUP(A:A,Sheet1!A:F,6,FALSE)</f>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26">
+        <f>VLOOKUP(A:A,Sheet1!A:F,5,FALSE)</f>
+        <v>2002</v>
+      </c>
+      <c r="C26" t="str">
+        <f>VLOOKUP(A:A,Sheet1!A:F,6,FALSE)</f>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>33</v>
+      </c>
+      <c r="B27">
+        <f>VLOOKUP(A:A,Sheet1!A:F,5,FALSE)</f>
+        <v>1998</v>
+      </c>
+      <c r="C27" t="str">
+        <f>VLOOKUP(A:A,Sheet1!A:F,6,FALSE)</f>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>35</v>
+      </c>
+      <c r="B28">
+        <f>VLOOKUP(A:A,Sheet1!A:F,5,FALSE)</f>
+        <v>1995</v>
+      </c>
+      <c r="C28" t="str">
+        <f>VLOOKUP(A:A,Sheet1!A:F,6,FALSE)</f>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>36</v>
+      </c>
+      <c r="B29">
+        <f>VLOOKUP(A:A,Sheet1!A:F,5,FALSE)</f>
+        <v>1994</v>
+      </c>
+      <c r="C29" t="str">
+        <f>VLOOKUP(A:A,Sheet1!A:F,6,FALSE)</f>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>37</v>
+      </c>
+      <c r="B30">
+        <f>VLOOKUP(A:A,Sheet1!A:F,5,FALSE)</f>
+        <v>1994</v>
+      </c>
+      <c r="C30" t="str">
+        <f>VLOOKUP(A:A,Sheet1!A:F,6,FALSE)</f>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>40</v>
+      </c>
+      <c r="B31">
+        <f>VLOOKUP(A:A,Sheet1!A:F,5,FALSE)</f>
+        <v>1991</v>
+      </c>
+      <c r="C31" t="str">
+        <f>VLOOKUP(A:A,Sheet1!A:F,6,FALSE)</f>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>45</v>
+      </c>
+      <c r="B32">
+        <f>VLOOKUP(A:A,Sheet1!A:F,5,FALSE)</f>
+        <v>1985</v>
+      </c>
+      <c r="C32" t="str">
+        <f>VLOOKUP(A:A,Sheet1!A:F,6,FALSE)</f>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>47</v>
+      </c>
+      <c r="B33">
+        <f>VLOOKUP(A:A,Sheet1!A:F,5,FALSE)</f>
+        <v>1984</v>
+      </c>
+      <c r="C33" t="str">
+        <f>VLOOKUP(A:A,Sheet1!A:F,6,FALSE)</f>
+        <v>Late Dylan</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>52</v>
+      </c>
+      <c r="B34">
+        <f>VLOOKUP(A:A,Sheet1!A:F,5,FALSE)</f>
+        <v>1979</v>
+      </c>
+      <c r="C34" t="str">
+        <f>VLOOKUP(A:A,Sheet1!A:F,6,FALSE)</f>
+        <v>Early Dylan</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>54</v>
+      </c>
+      <c r="B35">
+        <f>VLOOKUP(A:A,Sheet1!A:F,5,FALSE)</f>
+        <v>1978</v>
+      </c>
+      <c r="C35" t="str">
+        <f>VLOOKUP(A:A,Sheet1!A:F,6,FALSE)</f>
+        <v>Early Dylan</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>55</v>
+      </c>
+      <c r="B36">
+        <f>VLOOKUP(A:A,Sheet1!A:F,5,FALSE)</f>
+        <v>1976</v>
+      </c>
+      <c r="C36" t="str">
+        <f>VLOOKUP(A:A,Sheet1!A:F,6,FALSE)</f>
+        <v>Early Dylan</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>59</v>
+      </c>
+      <c r="B37">
+        <f>VLOOKUP(A:A,Sheet1!A:F,5,FALSE)</f>
+        <v>1973</v>
+      </c>
+      <c r="C37" t="str">
+        <f>VLOOKUP(A:A,Sheet1!A:F,6,FALSE)</f>
+        <v>Early Dylan</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>61</v>
+      </c>
+      <c r="B38">
+        <f>VLOOKUP(A:A,Sheet1!A:F,5,FALSE)</f>
+        <v>1971</v>
+      </c>
+      <c r="C38" t="str">
+        <f>VLOOKUP(A:A,Sheet1!A:F,6,FALSE)</f>
+        <v>Early Dylan</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>66</v>
+      </c>
+      <c r="B39">
+        <f>VLOOKUP(A:A,Sheet1!A:F,5,FALSE)</f>
+        <v>1967</v>
+      </c>
+      <c r="C39" t="str">
+        <f>VLOOKUP(A:A,Sheet1!A:F,6,FALSE)</f>
+        <v>Early Dylan</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>70</v>
+      </c>
+      <c r="B40">
+        <f>VLOOKUP(A:A,Sheet1!A:F,5,FALSE)</f>
+        <v>1964</v>
+      </c>
+      <c r="C40" t="str">
+        <f>VLOOKUP(A:A,Sheet1!A:F,6,FALSE)</f>
+        <v>Early Dylan</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>74</v>
+      </c>
+      <c r="B41">
+        <v>1966</v>
+      </c>
+      <c r="C41" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>75</v>
+      </c>
+      <c r="B42">
+        <v>1997</v>
+      </c>
+      <c r="C42" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>76</v>
+      </c>
+      <c r="B43">
+        <v>1997</v>
+      </c>
+      <c r="C43" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>77</v>
+      </c>
+      <c r="B44">
+        <v>1975</v>
+      </c>
+      <c r="C44" t="s">
+        <v>81</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added viz.html and more data
</commit_message>
<xml_diff>
--- a/data/albumdata.xlsx
+++ b/data/albumdata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sammo\OneDrive\Desktop\digit494\bobdylan494\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2DF9B0F-6311-4075-9899-71B423A7BD16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BB8370F-78DB-4E2B-BC6F-C22A0C36410C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{FEEBB7A0-F159-473C-BB2C-0727624CED14}"/>
   </bookViews>
@@ -23,7 +23,7 @@
   </externalReferences>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="21" r:id="rId6"/>
+    <pivotCache cacheId="77" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -380,7 +380,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -388,7 +388,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2468,7 +2467,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E9FAE770-6282-4CD1-BB9D-4676A45A238F}" name="PivotTable2" cacheId="21" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E9FAE770-6282-4CD1-BB9D-4676A45A238F}" name="PivotTable2" cacheId="77" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B6" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="4">
     <pivotField showAll="0">
@@ -5394,7 +5393,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF024E5E-2B60-4CCD-9AEA-0C47E1324E06}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -5422,7 +5423,7 @@
       <c r="A4" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4">
         <v>21</v>
       </c>
     </row>
@@ -5430,7 +5431,7 @@
       <c r="A5" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5">
         <v>13</v>
       </c>
     </row>
@@ -5438,7 +5439,7 @@
       <c r="A6" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6">
         <v>34</v>
       </c>
     </row>

</xml_diff>